<commit_message>
reviewing notification,system constrains,id constrains and admin constrains
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_REVIEWS-SHEET.xlsx
+++ b/LH_REVIEWS/LH_REVIEWS-SHEET.xlsx
@@ -1,18 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28801"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{35B6EDC7-908D-46BB-A75F-568B0A6904B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="PMP" sheetId="3" r:id="rId1"/>
     <sheet name="SIQ" sheetId="4" r:id="rId2"/>
     <sheet name="CRS" sheetId="5" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="30">
   <si>
     <t>ID</t>
   </si>
@@ -105,12 +104,58 @@
   <si>
     <t>open</t>
   </si>
+  <si>
+    <t>LH_REVIEW_CRS_001</t>
+  </si>
+  <si>
+    <t>Ahmed Abuzaid</t>
+  </si>
+  <si>
+    <t>0ca4136</t>
+  </si>
+  <si>
+    <t>1_the sheet name is named sheet 1
+2_the feature column not useful in this case</t>
+  </si>
+  <si>
+    <t>omar sherif</t>
+  </si>
+  <si>
+    <t>LH_REVIEW_CRS_002</t>
+  </si>
+  <si>
+    <t>for the CRS item LH_CRS_005 – System Constrain, the current phrasing 
+“web-based system/PC based” is a bit unclear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">can you make it more clear </t>
+  </si>
+  <si>
+    <t>1_name the sheet according naming 
+convetion "LH_CRS"
+2_we can suffice with the feature name in the id</t>
+  </si>
+  <si>
+    <t>LH_REVIEW_CRS_003</t>
+  </si>
+  <si>
+    <t>LH_REVIEW_CRS_004</t>
+  </si>
+  <si>
+    <t>no comment on " LH_CRS_ID-CONSTRAINS_006"</t>
+  </si>
+  <si>
+    <t>no comment on "LH_CRS_ADMIN-CONSTRAINS_007"</t>
+  </si>
+  <si>
+    <t>no action</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -442,22 +487,22 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
+        <left style="thin">
           <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
       <border outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
@@ -640,22 +685,22 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
+        <left style="thin">
           <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
       <border outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
@@ -838,6 +883,15 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -845,15 +899,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -901,51 +946,51 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:H12" totalsRowShown="0" headerRowDxfId="35" headerRowBorderDxfId="33" tableBorderDxfId="34" totalsRowBorderDxfId="32">
-  <autoFilter ref="A1:H12" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:H12" totalsRowShown="0" headerRowDxfId="35" headerRowBorderDxfId="34" tableBorderDxfId="33" totalsRowBorderDxfId="32">
+  <autoFilter ref="A1:H12"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="31"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Reviewer" dataDxfId="30"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Version" dataDxfId="29"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Review Comments" dataDxfId="28"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Actions" dataDxfId="27"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Owner" dataDxfId="26"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Status" dataDxfId="25"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Reviewer verification" dataDxfId="24"/>
+    <tableColumn id="1" name="ID" dataDxfId="31"/>
+    <tableColumn id="2" name="Reviewer" dataDxfId="30"/>
+    <tableColumn id="3" name="Version" dataDxfId="29"/>
+    <tableColumn id="4" name="Review Comments" dataDxfId="28"/>
+    <tableColumn id="5" name="Actions" dataDxfId="27"/>
+    <tableColumn id="6" name="Owner" dataDxfId="26"/>
+    <tableColumn id="7" name="Status" dataDxfId="25"/>
+    <tableColumn id="8" name="Reviewer verification" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table24" displayName="Table24" ref="A1:H12" totalsRowShown="0" headerRowDxfId="23" headerRowBorderDxfId="21" tableBorderDxfId="22" totalsRowBorderDxfId="20">
-  <autoFilter ref="A1:H12" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table24" displayName="Table24" ref="A1:H12" totalsRowShown="0" headerRowDxfId="23" headerRowBorderDxfId="22" tableBorderDxfId="21" totalsRowBorderDxfId="20">
+  <autoFilter ref="A1:H12"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="ID" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Reviewer" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Version" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Review Comments" dataDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Actions" dataDxfId="15"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Owner" dataDxfId="14"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Status" dataDxfId="13"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Reviewer verification" dataDxfId="12"/>
+    <tableColumn id="1" name="ID" dataDxfId="19"/>
+    <tableColumn id="2" name="Reviewer" dataDxfId="18"/>
+    <tableColumn id="3" name="Version" dataDxfId="17"/>
+    <tableColumn id="4" name="Review Comments" dataDxfId="16"/>
+    <tableColumn id="5" name="Actions" dataDxfId="15"/>
+    <tableColumn id="6" name="Owner" dataDxfId="14"/>
+    <tableColumn id="7" name="Status" dataDxfId="13"/>
+    <tableColumn id="8" name="Reviewer verification" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table245" displayName="Table245" ref="A1:H12" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="9" tableBorderDxfId="10" totalsRowBorderDxfId="8">
-  <autoFilter ref="A1:H12" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table245" displayName="Table245" ref="A1:H12" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
+  <autoFilter ref="A1:H12"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="ID" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Reviewer" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Version" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Review Comments" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Actions" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Owner" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Status" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Reviewer verification" dataDxfId="0"/>
+    <tableColumn id="1" name="ID" dataDxfId="7"/>
+    <tableColumn id="2" name="Reviewer" dataDxfId="6"/>
+    <tableColumn id="3" name="Version" dataDxfId="5"/>
+    <tableColumn id="4" name="Review Comments" dataDxfId="4"/>
+    <tableColumn id="5" name="Actions" dataDxfId="3"/>
+    <tableColumn id="6" name="Owner" dataDxfId="2"/>
+    <tableColumn id="7" name="Status" dataDxfId="1"/>
+    <tableColumn id="8" name="Reviewer verification" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1213,14 +1258,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" customWidth="1"/>
@@ -1231,7 +1276,7 @@
     <col min="8" max="8" width="30.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="10" customFormat="1" ht="18.75">
+    <row r="1" spans="1:8" s="10" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1257,7 +1302,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1267,7 +1312,7 @@
       <c r="G2" s="1"/>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1277,7 +1322,7 @@
       <c r="G3" s="1"/>
       <c r="H3" s="5"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1287,7 +1332,7 @@
       <c r="G4" s="1"/>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1297,7 +1342,7 @@
       <c r="G5" s="1"/>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -1307,7 +1352,7 @@
       <c r="G6" s="1"/>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1317,7 +1362,7 @@
       <c r="G7" s="1"/>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1327,7 +1372,7 @@
       <c r="G8" s="1"/>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1337,7 +1382,7 @@
       <c r="G9" s="1"/>
       <c r="H9" s="5"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1347,7 +1392,7 @@
       <c r="G10" s="1"/>
       <c r="H10" s="5"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1357,7 +1402,7 @@
       <c r="G11" s="1"/>
       <c r="H11" s="5"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -1369,10 +1414,10 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from list" sqref="G2:G12" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from list" sqref="G2:G12">
       <formula1>"open,in progress,closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from list" sqref="H2:H12" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from list" sqref="H2:H12">
       <formula1>"open,closed"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1384,14 +1429,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
@@ -1403,7 +1448,7 @@
     <col min="8" max="8" width="30.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="10" customFormat="1" ht="18.75">
+    <row r="1" spans="1:8" s="10" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1429,7 +1474,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="409.6">
+    <row r="2" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -1455,7 +1500,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1465,7 +1510,7 @@
       <c r="G3" s="1"/>
       <c r="H3" s="5"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1475,7 +1520,7 @@
       <c r="G4" s="1"/>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1485,7 +1530,7 @@
       <c r="G5" s="1"/>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -1495,7 +1540,7 @@
       <c r="G6" s="1"/>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1505,7 +1550,7 @@
       <c r="G7" s="1"/>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1515,7 +1560,7 @@
       <c r="G8" s="1"/>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1525,7 +1570,7 @@
       <c r="G9" s="1"/>
       <c r="H9" s="5"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1535,7 +1580,7 @@
       <c r="G10" s="1"/>
       <c r="H10" s="5"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1545,7 +1590,7 @@
       <c r="G11" s="1"/>
       <c r="H11" s="5"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -1557,10 +1602,10 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from list" sqref="H2:H12" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from list" sqref="H2:H12">
       <formula1>"open,closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from list" sqref="G2:G12" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from list" sqref="G2:G12">
       <formula1>"open,in progress,closed"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1572,26 +1617,26 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" customWidth="1"/>
-    <col min="4" max="4" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.7109375" customWidth="1"/>
+    <col min="5" max="5" width="46.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="30.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="10" customFormat="1" ht="18.75">
+    <row r="1" spans="1:8" s="10" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1617,13 +1662,25 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="4"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
+    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="G2" s="1" t="s">
         <v>15</v>
       </c>
@@ -1631,37 +1688,85 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="4"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="5"/>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="4"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="5"/>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="4"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="5"/>
-    </row>
-    <row r="6" spans="1:8">
+    <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -1671,7 +1776,7 @@
       <c r="G6" s="1"/>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1681,7 +1786,7 @@
       <c r="G7" s="1"/>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1691,7 +1796,7 @@
       <c r="G8" s="1"/>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1701,7 +1806,7 @@
       <c r="G9" s="1"/>
       <c r="H9" s="5"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1711,7 +1816,7 @@
       <c r="G10" s="1"/>
       <c r="H10" s="5"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1721,7 +1826,7 @@
       <c r="G11" s="1"/>
       <c r="H11" s="5"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -1733,16 +1838,17 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from list" sqref="G2:G12" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from list" sqref="G2:G12">
       <formula1>"open,in progress,closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from list" sqref="H2:H12" xr:uid="{00000000-0002-0000-0200-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from list" sqref="H2:H12">
       <formula1>"open,closed"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
verify reviews on notifications and constrains plus adding date section to review sheet
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_REVIEWS-SHEET.xlsx
+++ b/LH_REVIEWS/LH_REVIEWS-SHEET.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEF9DCD3-DB0B-4893-AFEC-34D16E0AFA4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="PMP" sheetId="3" r:id="rId1"/>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="34">
   <si>
     <t>ID</t>
   </si>
@@ -149,12 +148,15 @@
   <si>
     <t>Update all IDs to replace underscores (_) with hyphens (-) to ensure compliance with the PMP format guidelines.</t>
   </si>
+  <si>
+    <t>date</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -176,16 +178,36 @@
       <name val="Calibri"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -304,11 +326,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
@@ -338,9 +390,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -365,6 +414,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -978,42 +1036,42 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:H12" totalsRowShown="0" headerRowDxfId="35" headerRowBorderDxfId="34" tableBorderDxfId="33" totalsRowBorderDxfId="32">
-  <autoFilter ref="A1:H12" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:H12" totalsRowShown="0" headerRowDxfId="35" headerRowBorderDxfId="34" tableBorderDxfId="33" totalsRowBorderDxfId="32">
+  <autoFilter ref="A1:H12"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="31"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Reviewer" dataDxfId="30"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Version" dataDxfId="29"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Review Comments" dataDxfId="28"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Actions" dataDxfId="27"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Owner" dataDxfId="26"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Status" dataDxfId="25"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Reviewer verification" dataDxfId="24"/>
+    <tableColumn id="1" name="ID" dataDxfId="31"/>
+    <tableColumn id="2" name="Reviewer" dataDxfId="30"/>
+    <tableColumn id="3" name="Version" dataDxfId="29"/>
+    <tableColumn id="4" name="Review Comments" dataDxfId="28"/>
+    <tableColumn id="5" name="Actions" dataDxfId="27"/>
+    <tableColumn id="6" name="Owner" dataDxfId="26"/>
+    <tableColumn id="7" name="Status" dataDxfId="25"/>
+    <tableColumn id="8" name="Reviewer verification" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table24" displayName="Table24" ref="A1:H12" totalsRowShown="0" headerRowDxfId="23" headerRowBorderDxfId="22" tableBorderDxfId="21" totalsRowBorderDxfId="20">
-  <autoFilter ref="A1:H12" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table24" displayName="Table24" ref="A1:H12" totalsRowShown="0" headerRowDxfId="23" headerRowBorderDxfId="22" tableBorderDxfId="21" totalsRowBorderDxfId="20">
+  <autoFilter ref="A1:H12"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="ID" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Reviewer" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Version" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Review Comments" dataDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Actions" dataDxfId="15"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Owner" dataDxfId="14"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Status" dataDxfId="13"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Reviewer verification" dataDxfId="12"/>
+    <tableColumn id="1" name="ID" dataDxfId="19"/>
+    <tableColumn id="2" name="Reviewer" dataDxfId="18"/>
+    <tableColumn id="3" name="Version" dataDxfId="17"/>
+    <tableColumn id="4" name="Review Comments" dataDxfId="16"/>
+    <tableColumn id="5" name="Actions" dataDxfId="15"/>
+    <tableColumn id="6" name="Owner" dataDxfId="14"/>
+    <tableColumn id="7" name="Status" dataDxfId="13"/>
+    <tableColumn id="8" name="Reviewer verification" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table245" displayName="Table245" ref="A1:H13" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
-  <autoFilter ref="A1:H13" xr:uid="{00000000-0009-0000-0100-000004000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table245" displayName="Table245" ref="B1:I13" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
+  <autoFilter ref="B1:I13">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -1021,14 +1079,14 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="ID" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Reviewer" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Version" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Review Comments" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Actions" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Owner" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Status" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Reviewer verification" dataDxfId="0"/>
+    <tableColumn id="1" name="ID" dataDxfId="7"/>
+    <tableColumn id="2" name="Reviewer" dataDxfId="6"/>
+    <tableColumn id="3" name="Version" dataDxfId="5"/>
+    <tableColumn id="4" name="Review Comments" dataDxfId="4"/>
+    <tableColumn id="5" name="Actions" dataDxfId="3"/>
+    <tableColumn id="6" name="Owner" dataDxfId="2"/>
+    <tableColumn id="7" name="Status" dataDxfId="1"/>
+    <tableColumn id="8" name="Reviewer verification" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1296,25 +1354,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" customWidth="1"/>
-    <col min="4" max="4" width="27.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="10" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" s="10" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1340,7 +1398,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1350,7 +1408,7 @@
       <c r="G2" s="1"/>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1360,7 +1418,7 @@
       <c r="G3" s="1"/>
       <c r="H3" s="5"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1370,7 +1428,7 @@
       <c r="G4" s="1"/>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1380,7 +1438,7 @@
       <c r="G5" s="1"/>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -1390,7 +1448,7 @@
       <c r="G6" s="1"/>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1400,7 +1458,7 @@
       <c r="G7" s="1"/>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1410,7 +1468,7 @@
       <c r="G8" s="1"/>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1420,7 +1478,7 @@
       <c r="G9" s="1"/>
       <c r="H9" s="5"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1430,7 +1488,7 @@
       <c r="G10" s="1"/>
       <c r="H10" s="5"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1440,7 +1498,7 @@
       <c r="G11" s="1"/>
       <c r="H11" s="5"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -1452,10 +1510,10 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from list" sqref="G2:G12" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from list" sqref="G2:G12">
       <formula1>"open,in progress,closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from list" sqref="H2:H12" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from list" sqref="H2:H12">
       <formula1>"open,closed"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1467,26 +1525,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" customWidth="1"/>
-    <col min="4" max="4" width="36.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" customWidth="1"/>
+    <col min="4" max="4" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="10" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" s="10" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1512,7 +1570,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -1538,7 +1596,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1548,7 +1606,7 @@
       <c r="G3" s="1"/>
       <c r="H3" s="5"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1558,7 +1616,7 @@
       <c r="G4" s="1"/>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1568,7 +1626,7 @@
       <c r="G5" s="1"/>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -1578,7 +1636,7 @@
       <c r="G6" s="1"/>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1588,7 +1646,7 @@
       <c r="G7" s="1"/>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1598,7 +1656,7 @@
       <c r="G8" s="1"/>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1608,7 +1666,7 @@
       <c r="G9" s="1"/>
       <c r="H9" s="5"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1618,7 +1676,7 @@
       <c r="G10" s="1"/>
       <c r="H10" s="5"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1628,7 +1686,7 @@
       <c r="G11" s="1"/>
       <c r="H11" s="5"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -1640,10 +1698,10 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from list" sqref="H2:H12" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from list" sqref="H2:H12">
       <formula1>"open,closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from list" sqref="G2:G12" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from list" sqref="G2:G12">
       <formula1>"open,in progress,closed"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1655,278 +1713,306 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.44140625" style="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.88671875" style="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5546875" style="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="61.109375" style="23" customWidth="1"/>
-    <col min="5" max="5" width="46.5546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5546875" style="22" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13" style="22" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.88671875" style="22" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="22"/>
+    <col min="1" max="1" width="8.85546875" style="21"/>
+    <col min="2" max="2" width="19.42578125" style="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" style="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="61.140625" style="22" customWidth="1"/>
+    <col min="6" max="6" width="46.5703125" style="22" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" style="21" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13" style="21" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.85546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.85546875" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:9" s="18" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="C1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="D1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="E1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="F1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="G1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="H1" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="I1" s="17" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="20" t="s">
+    <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="24">
+        <v>45873</v>
+      </c>
+      <c r="B2" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="C2" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="D2" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="E2" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="F2" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="G2" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="H2" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="21" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="20" t="s">
+      <c r="I2" s="20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="25">
+        <v>45873</v>
+      </c>
+      <c r="B3" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="C3" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="D3" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="E3" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="F3" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="G3" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="H3" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="21" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="20" t="s">
+      <c r="I3" s="20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="24">
+        <v>45873</v>
+      </c>
+      <c r="B4" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="C4" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="D4" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="E4" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="F4" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="G4" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="H4" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="21" t="s">
+      <c r="I4" s="20" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="20" t="s">
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="25">
+        <v>45873</v>
+      </c>
+      <c r="B5" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="C5" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="D5" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="E5" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="F5" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="G5" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="H5" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="21" t="s">
+      <c r="I5" s="20" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="4"/>
-      <c r="B6" s="1"/>
+    <row r="6" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="19"/>
+      <c r="B6" s="4"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
-      <c r="H6" s="5"/>
-    </row>
-    <row r="7" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="4"/>
-      <c r="B7" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="5"/>
+    </row>
+    <row r="7" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="19"/>
+      <c r="B7" s="4"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
-      <c r="H7" s="5"/>
-    </row>
-    <row r="8" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="4"/>
-      <c r="B8" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="5"/>
+    </row>
+    <row r="8" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="19"/>
+      <c r="B8" s="4"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-      <c r="H8" s="5"/>
-    </row>
-    <row r="9" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="4"/>
-      <c r="B9" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="5"/>
+    </row>
+    <row r="9" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="19"/>
+      <c r="B9" s="4"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="5"/>
-    </row>
-    <row r="10" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="4"/>
-      <c r="B10" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="5"/>
+    </row>
+    <row r="10" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="19"/>
+      <c r="B10" s="4"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
-      <c r="H10" s="5"/>
-    </row>
-    <row r="11" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="4"/>
-      <c r="B11" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="5"/>
+    </row>
+    <row r="11" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="19"/>
+      <c r="B11" s="4"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
-      <c r="H11" s="5"/>
-    </row>
-    <row r="12" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="3"/>
-      <c r="B12" s="6"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="5"/>
+    </row>
+    <row r="12" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="19"/>
+      <c r="B12" s="3"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
-      <c r="H12" s="2"/>
-    </row>
-    <row r="13" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A13" s="20" t="s">
+      <c r="H12" s="6"/>
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="24">
+        <v>45873</v>
+      </c>
+      <c r="B13" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="C13" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="D13" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="E13" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="F13" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="F13" s="14" t="s">
+      <c r="G13" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="G13" s="14" t="s">
+      <c r="H13" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="H13" s="21" t="s">
+      <c r="I13" s="20" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="20"/>
-      <c r="B14" s="14"/>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="19"/>
+      <c r="B14" s="19"/>
       <c r="C14" s="14"/>
-      <c r="D14" s="13"/>
+      <c r="D14" s="14"/>
       <c r="E14" s="13"/>
-      <c r="F14" s="14"/>
+      <c r="F14" s="13"/>
       <c r="G14" s="14"/>
-      <c r="H14" s="21"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="20"/>
-      <c r="B15" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="20"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="19"/>
+      <c r="B15" s="19"/>
       <c r="C15" s="14"/>
-      <c r="D15" s="13"/>
+      <c r="D15" s="14"/>
       <c r="E15" s="13"/>
-      <c r="F15" s="14"/>
+      <c r="F15" s="13"/>
       <c r="G15" s="14"/>
-      <c r="H15" s="21"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="20"/>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from list" sqref="G2:G13" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from list" sqref="H2:H13">
       <formula1>"open,in progress,closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from list" sqref="H2:H13" xr:uid="{00000000-0002-0000-0200-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from list" sqref="I2:I13">
       <formula1>"open,closed"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
"Updated review sheet, added PMP Review
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_REVIEWS-SHEET.xlsx
+++ b/LH_REVIEWS/LH_REVIEWS-SHEET.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="PMP" sheetId="3" r:id="rId1"/>
     <sheet name="SIQ" sheetId="4" r:id="rId2"/>
     <sheet name="CRS" sheetId="5" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="72">
   <si>
     <t>ID</t>
   </si>
@@ -149,14 +149,223 @@
     <t>Update all IDs to replace underscores (_) with hyphens (-) to ensure compliance with the PMP format guidelines.</t>
   </si>
   <si>
-    <t>date</t>
+    <t>LH_REVIEW_PMP_001</t>
+  </si>
+  <si>
+    <t>Eman Abusalim</t>
+  </si>
+  <si>
+    <t>Gehad Ashry</t>
+  </si>
+  <si>
+    <t>LH_REVIEW_PMP_002</t>
+  </si>
+  <si>
+    <t>LH_REVIEW_PMP_003</t>
+  </si>
+  <si>
+    <t>LH_REVIEW_PMP_004</t>
+  </si>
+  <si>
+    <t>LH_REVIEW_PMP_005</t>
+  </si>
+  <si>
+    <t>LH_REVIEW_PMP_006</t>
+  </si>
+  <si>
+    <t>LH_REVIEW_PMP_007</t>
+  </si>
+  <si>
+    <t>LH_REVIEW_PMP_008</t>
+  </si>
+  <si>
+    <t>LH_REVIEW_PMP_009</t>
+  </si>
+  <si>
+    <t>LH_REVIEW_PMP_010</t>
+  </si>
+  <si>
+    <t>LH_REVIEW_PMP_011</t>
+  </si>
+  <si>
+    <t>the version history section is currently empty. 
+This section is essential for tracking changes to the Project Management Plan over time.</t>
+  </si>
+  <si>
+    <t>Please fill in at least the intial version and the authr and 
+the date of creation .</t>
+  </si>
+  <si>
+    <t>Please consider rearranging these sections so that the 'Table of Contents' comes first.
+ This will help readers quickly understand the structure of the document upon opening it.</t>
+  </si>
+  <si>
+    <t>The 'Version History' section appears before the listed 'Table of Contents', although 
+                   it is listed as one of the content items</t>
+  </si>
+  <si>
+    <t>The objective section provides a clear overall picture of the project, which is great. 
+However, it currently lacks the SMART criteria.</t>
+  </si>
+  <si>
+    <t>To strengthen it, consider breaking it down into specific, measurable goals with defined deadlines that reflect the key features of the platform.</t>
+  </si>
+  <si>
+    <t>The current Reporting Process Flow presents a basic outline of the reporting stages.
+ However, the steps need more detail regarding responsibilities, timing, communication channels, and tools used to ensure a smooth and consistent reporting cycle.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Please consider expanding each step  of thr reporting process flow
+for better clarity and execution.</t>
+  </si>
+  <si>
+    <t>please make the link redirect to the Configuration Item List so that the reader can easly get the 2- Configuration Items (CI)</t>
+  </si>
+  <si>
+    <t>The work out of scope is writdoten very well howeverwe need to be more 
+spacific about activites we will do</t>
+  </si>
+  <si>
+    <t>Add the following :
+ -unit testing 
+-Desktop application
+-Application programming interface</t>
+  </si>
+  <si>
+    <t>in the Project Scope section, the line "Users can follow categories and engage with the content"is too broad and may cause confusion regarding the actual features of the system.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It is recommended to revise this statement to: "Users can follow categories and receive updates for new content."
+This alternative better aligns with the defined features in the scope and avoids implying unsupported interactions such as commenting, liking, or sharing.
+</t>
+  </si>
+  <si>
+    <t>In the configuration management plan section
+The Hyberlink in the configuration items is not clickable</t>
+  </si>
+  <si>
+    <t>It is recommended to confirm the expected admin capabilities with the customer before finalizing the scop</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">he scope item </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Admin Features: Admins will have control over content management and user moderation"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 
+may need clarification. 
+The current plan assumes that the admin's only action is to delete content, but this was not specified by the customer.</t>
+    </r>
+  </si>
+  <si>
+    <t>he matrix uses the abbreviation 'RICARS,' which appears to be a typographical error. 
+The correct acronym is 'RASIC.'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The matrix should be updated to reflect the proper roles of Responsible, Accountable, Support, Informed, and Consulted. Please revise the matrix for accuracy and clarity."
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There seems to be a conflict between the "Out of Work Scope" section and the "Work Breakdown Structure" (WBS). 
+The "Out of Work Scope" lists "Integration with external content providers or third-party databases" as excluded, which suggests that the project will not involve external integrations. 
+However, in the WBS, the tasks "Define system and database architecture" and "Develop business logic and database integration" are included, which might imply integration with external databases or services.
+</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Please clarify in the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>WBS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> that the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"database integration"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> refers to internal system/database integration and not external content providers, as this will align with the stated project scope.
+ If any external integrations are planned, they should be explicitly mentioned as part of the scope or excluded from the WBS accordingly.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">After reviewing the Communication Matrix, I suggest modifying the frequency for the Risk Updates and Progress Reporting  sections.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Both of these communication goals could be set to "As Needed" rather than weekly, to ensure that updates are only provided 
+when there is significant progress or risk-related developments that require stakeholder attention.
+ This would help in keeping the communication focused and relevant.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It should be noted that the team standup meetings occur on Saturday, Monday, and Wednesday, rather than daily.
+ This adjustment will provide a clearer understanding of the actual meeting schedule and help ensure proper communication flow among team members.
+</t>
+  </si>
+  <si>
+    <t>LH_REVIEW_PMP_012</t>
+  </si>
+  <si>
+    <t>V1.0</t>
+  </si>
+  <si>
+    <t>v1.0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -179,35 +388,31 @@
       <charset val="1"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="14"/>
-      <color theme="0"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor theme="4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor theme="4" tint="0.79998168889431442"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="12">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -326,41 +531,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
@@ -390,6 +565,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -414,14 +592,50 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1010,7 +1224,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -1036,8 +1250,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:H12" totalsRowShown="0" headerRowDxfId="35" headerRowBorderDxfId="34" tableBorderDxfId="33" totalsRowBorderDxfId="32">
-  <autoFilter ref="A1:H12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:H41" totalsRowShown="0" headerRowDxfId="35" headerRowBorderDxfId="34" tableBorderDxfId="33" totalsRowBorderDxfId="32">
+  <autoFilter ref="A1:H41"/>
   <tableColumns count="8">
     <tableColumn id="1" name="ID" dataDxfId="31"/>
     <tableColumn id="2" name="Reviewer" dataDxfId="30"/>
@@ -1070,8 +1284,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table245" displayName="Table245" ref="B1:I13" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
-  <autoFilter ref="B1:I13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table245" displayName="Table245" ref="A1:H13" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
+  <autoFilter ref="A1:H13">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -1135,7 +1349,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1170,7 +1384,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1347,7 +1561,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1355,165 +1569,620 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="31.5703125" customWidth="1"/>
     <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" customWidth="1"/>
-    <col min="4" max="4" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+    <col min="4" max="4" width="82.7109375" customWidth="1"/>
+    <col min="5" max="5" width="66.85546875" customWidth="1"/>
     <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="30.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="10" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:8" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="18" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="5"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="5"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="5"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="5"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="5"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="5"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="5"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="5"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
+    <row r="2" spans="1:8" s="27" customFormat="1" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="26"/>
+    </row>
+    <row r="3" spans="1:8" s="32" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="31"/>
+    </row>
+    <row r="4" spans="1:8" s="32" customFormat="1" ht="81" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="31"/>
+    </row>
+    <row r="5" spans="1:8" s="32" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="31"/>
+    </row>
+    <row r="6" spans="1:8" s="32" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="31"/>
+    </row>
+    <row r="7" spans="1:8" s="32" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="31"/>
+    </row>
+    <row r="8" spans="1:8" s="32" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A8" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="F8" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="31"/>
+    </row>
+    <row r="9" spans="1:8" s="27" customFormat="1" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="E9" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="F9" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="26"/>
+    </row>
+    <row r="10" spans="1:8" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="F10" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="G10" s="25" t="s">
+        <v>15</v>
+      </c>
       <c r="H10" s="5"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="5"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="2"/>
+    <row r="11" spans="1:8" s="32" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="F11" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" s="31"/>
+    </row>
+    <row r="12" spans="1:8" s="34" customFormat="1" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="37" t="s">
+        <v>66</v>
+      </c>
+      <c r="E12" s="37" t="s">
+        <v>67</v>
+      </c>
+      <c r="F12" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="G12" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" s="38"/>
+    </row>
+    <row r="13" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13" s="6"/>
+      <c r="F13" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="G13" s="6"/>
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="5"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="5"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="5"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="5"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="5"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="5"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="5"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="4"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="28"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="5"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="4"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="5"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="4"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="28"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="5"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="4"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="28"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="5"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="4"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="5"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="4"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="5"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="4"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="28"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="5"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="4"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="28"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="5"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="4"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="5"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="4"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="5"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="4"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="5"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="4"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="28"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="5"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="4"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="28"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="5"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="4"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="28"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="5"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="4"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="28"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="5"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="4"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="28"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="5"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="4"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="28"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="5"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="4"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="28"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="5"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="4"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="28"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="5"/>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from list" sqref="G2:G12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from list" sqref="G2:G41">
       <formula1>"open,in progress,closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from list" sqref="H2:H12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from list" sqref="H2:H41">
       <formula1>"open,closed"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1528,7 +2197,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1714,305 +2383,277 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="21"/>
-    <col min="2" max="2" width="19.42578125" style="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" style="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" style="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="61.140625" style="22" customWidth="1"/>
-    <col min="6" max="6" width="46.5703125" style="22" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" style="21" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13" style="21" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.85546875" style="21" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.85546875" style="21"/>
+    <col min="1" max="1" width="19.42578125" style="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" style="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" style="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="61.140625" style="23" customWidth="1"/>
+    <col min="5" max="5" width="46.5703125" style="23" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" style="22" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13" style="22" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.85546875" style="22" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.85546875" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="18" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="15" t="s">
+    <row r="1" spans="1:8" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="C1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="D1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="E1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="F1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="G1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="H1" s="18" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="24">
-        <v>45873</v>
-      </c>
-      <c r="B2" s="19" t="s">
+    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
         <v>16</v>
       </c>
+      <c r="B2" s="14" t="s">
+        <v>17</v>
+      </c>
       <c r="C2" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="21" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="C3" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="14" t="s">
+      <c r="D3" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="G3" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="20" t="s">
+      <c r="H3" s="21" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="14" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="25">
-        <v>45873</v>
-      </c>
-      <c r="B3" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="14" t="s">
+      <c r="H4" s="21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="C5" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="14" t="s">
+      <c r="D5" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="G5" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="20" t="s">
+      <c r="H5" s="21" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="24">
-        <v>45873</v>
-      </c>
-      <c r="B4" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="H4" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="20" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="25">
-        <v>45873</v>
-      </c>
-      <c r="B5" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="H5" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" s="20" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="19"/>
-      <c r="B6" s="4"/>
+    <row r="6" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="5"/>
-    </row>
-    <row r="7" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="19"/>
-      <c r="B7" s="4"/>
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="5"/>
-    </row>
-    <row r="8" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="19"/>
-      <c r="B8" s="4"/>
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="5"/>
-    </row>
-    <row r="9" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="19"/>
-      <c r="B9" s="4"/>
+      <c r="H8" s="5"/>
+    </row>
+    <row r="9" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="5"/>
-    </row>
-    <row r="10" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="19"/>
-      <c r="B10" s="4"/>
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="5"/>
-    </row>
-    <row r="11" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="19"/>
-      <c r="B11" s="4"/>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="5"/>
-    </row>
-    <row r="12" spans="1:9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="19"/>
-      <c r="B12" s="3"/>
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" spans="1:8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" s="6"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="2"/>
-    </row>
-    <row r="13" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="24">
-        <v>45873</v>
-      </c>
-      <c r="B13" s="19" t="s">
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="20" t="s">
         <v>29</v>
       </c>
+      <c r="B13" s="14" t="s">
+        <v>30</v>
+      </c>
       <c r="C13" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="14" t="s">
         <v>18</v>
       </c>
+      <c r="D13" s="13" t="s">
+        <v>31</v>
+      </c>
       <c r="E13" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="F13" s="13" t="s">
         <v>32</v>
       </c>
+      <c r="F13" s="14" t="s">
+        <v>17</v>
+      </c>
       <c r="G13" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="H13" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="I13" s="20" t="s">
+      <c r="H13" s="21" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="19"/>
-      <c r="B14" s="19"/>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="20"/>
+      <c r="B14" s="14"/>
       <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
+      <c r="D14" s="13"/>
       <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
+      <c r="F14" s="14"/>
       <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="20"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="19"/>
-      <c r="B15" s="19"/>
+      <c r="H14" s="21"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="20"/>
+      <c r="B15" s="14"/>
       <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
+      <c r="D15" s="13"/>
       <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
+      <c r="F15" s="14"/>
       <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="20"/>
+      <c r="H15" s="21"/>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from list" sqref="H2:H13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from list" sqref="G2:G13">
       <formula1>"open,in progress,closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from list" sqref="I2:I13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from list" sqref="H2:H13">
       <formula1>"open,closed"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
verify the review on notifications and constrains
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_REVIEWS-SHEET.xlsx
+++ b/LH_REVIEWS/LH_REVIEWS-SHEET.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
-  <workbookPr filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="PMP" sheetId="3" r:id="rId1"/>
@@ -364,7 +364,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1561,7 +1561,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2197,7 +2197,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -2385,8 +2385,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2451,7 +2451,7 @@
         <v>14</v>
       </c>
       <c r="H2" s="21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2477,7 +2477,7 @@
         <v>14</v>
       </c>
       <c r="H3" s="21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">

</xml_diff>